<commit_message>
Added code & data from study 1
</commit_message>
<xml_diff>
--- a/data/clean/003_RPE-Data_stage-3.xlsx
+++ b/data/clean/003_RPE-Data_stage-3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t xml:space="preserve">Participant ID</t>
   </si>
@@ -165,6 +165,87 @@
   </si>
   <si>
     <t xml:space="preserve">drug use may be an outlet for different situations like homelesseness, trauma, hunger and poverty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobriety should be required for treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm sure sobriety will change to effectiveness of the drugs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People should be under the influence when starting medication.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think that people can be California sober. I don't think that you have to have complete sobriety to treat an addiction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some people can get over their addiction and maintain a good control over their addiction by just having a toke or drink or two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If sobriety is required, that leaves out many addicts who are unable to stop using drugs at any point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You must be clean (sober) in order to receive treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That doesn't make any sense. If sobriety was required for the treatment, they wouldn't need the treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It means that before they could be treated, they must be off drugs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The statement is confusing regarding the extent of sobriety.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if they were sober they wouldnt need treatment   thats not a valid statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you must be "clean" to come get "clean"    ?????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People who use drugs should be able to use medications used to treat addiction (buprenorphine, naltrexone, or methadone) for any length of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sounds reasonable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It means people going through detox should have access to this medication.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not one person is the same as another. As long as the addict is trying to stay clean, they should be allowed to do whatever it takes to get out of their addiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That addicts can have medications for as long as they need or want</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would also say  in addition to other treatments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the drugs are used for any length of time, the addiction is not being treated. The drug user is still using drugs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addicts should be able to use treatment drugs for as long as they like.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slightly disagree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those drugs should be used for a limited time to stop drug use, not as a replacement to these drugs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It means that these drugs should be used to replace the illicit hard drug use rather than as a means to stop drug use altogether.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is going to allow them to go back and forth from using to rehab   i understand people relapse but allowing them to harm themselves and the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an open ended supply of medication to users who want to get clean   i get that and yes its a good idea but at what cost   financially and to whos health    not all are criminals but some are   there has to be a balance</t>
   </si>
 </sst>
 </file>
@@ -852,6 +933,126 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -892,6 +1093,126 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>